<commit_message>
JS8 - Tugas 1-3_Supplier
</commit_message>
<xml_diff>
--- a/public/template_level.xlsx
+++ b/public/template_level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS_2024\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{335D5E84-D842-4A91-A96C-1FED2982FACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2852FE29-B1F3-4366-8205-514B2BB1A9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9420" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>level_kode</t>
   </si>
@@ -33,16 +33,10 @@
     <t>level_nama</t>
   </si>
   <si>
-    <t>BA</t>
+    <t>Developer</t>
   </si>
   <si>
-    <t>Brand Ambassador</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Chief Executive Officer</t>
+    <t>DEV</t>
   </si>
 </sst>
 </file>
@@ -403,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EC98B1-BB63-4991-9AD2-D5CD08BDE7D3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,18 +419,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>